<commit_message>
Compare timings RFLINK, Sonoff/Portisch and Broadlink RM with same signal
</commit_message>
<xml_diff>
--- a/samples/debugsorted1.xlsx
+++ b/samples/debugsorted1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\node\pulsespaceindex\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{CC4EC39E-3201-448C-BAAD-CD700814335E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7880289-B470-444B-9E37-D187B703D0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="debugsorted1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="441">
   <si>
     <t>Count</t>
   </si>
@@ -1348,7 +1359,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2188,14 +2199,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K300"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E293" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E287" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K129" sqref="K129"/>
+      <selection pane="bottomRight" activeCell="O290" sqref="O290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6240,7 +6251,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>125</v>
       </c>
@@ -6257,7 +6268,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>126</v>
       </c>
@@ -6280,7 +6291,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>126</v>
       </c>
@@ -6306,7 +6317,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>126</v>
       </c>
@@ -6332,7 +6343,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="197" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>126</v>
       </c>
@@ -6358,7 +6369,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>129</v>
       </c>
@@ -6375,7 +6386,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>129</v>
       </c>
@@ -6392,7 +6403,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>129</v>
       </c>
@@ -6409,7 +6420,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>131</v>
       </c>
@@ -6429,7 +6440,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>131</v>
       </c>
@@ -6449,7 +6460,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>132</v>
       </c>
@@ -6471,8 +6482,20 @@
       <c r="K203" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O203">
+        <f t="shared" ref="O203:O211" si="0">C203/B203</f>
+        <v>8.296551724137931</v>
+      </c>
+      <c r="P203">
+        <f t="shared" ref="P203:P211" si="1">D203/B203</f>
+        <v>18.620689655172413</v>
+      </c>
+      <c r="Q203">
+        <f>D203/C203</f>
+        <v>2.2443890274314215</v>
+      </c>
+    </row>
+    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>132</v>
       </c>
@@ -6494,8 +6517,20 @@
       <c r="K204" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O204">
+        <f t="shared" si="0"/>
+        <v>8.183673469387756</v>
+      </c>
+      <c r="P204">
+        <f t="shared" si="1"/>
+        <v>18.367346938775512</v>
+      </c>
+      <c r="Q204">
+        <f t="shared" ref="Q204:Q228" si="2">D204/C204</f>
+        <v>2.2443890274314215</v>
+      </c>
+    </row>
+    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>132</v>
       </c>
@@ -6517,8 +6552,20 @@
       <c r="K205" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O205">
+        <f t="shared" si="0"/>
+        <v>8.0653594771241828</v>
+      </c>
+      <c r="P205">
+        <f t="shared" si="1"/>
+        <v>17.058823529411764</v>
+      </c>
+      <c r="Q205">
+        <f t="shared" si="2"/>
+        <v>2.1150729335494329</v>
+      </c>
+    </row>
+    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>132</v>
       </c>
@@ -6540,8 +6587,20 @@
       <c r="K206" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O206">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="P206">
+        <f t="shared" si="1"/>
+        <v>16.948051948051948</v>
+      </c>
+      <c r="Q206">
+        <f t="shared" si="2"/>
+        <v>2.1185064935064934</v>
+      </c>
+    </row>
+    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>132</v>
       </c>
@@ -6563,8 +6622,20 @@
       <c r="K207" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O207">
+        <f t="shared" si="0"/>
+        <v>8.0129870129870131</v>
+      </c>
+      <c r="P207">
+        <f t="shared" si="1"/>
+        <v>16.948051948051948</v>
+      </c>
+      <c r="Q207">
+        <f t="shared" si="2"/>
+        <v>2.1150729335494329</v>
+      </c>
+    </row>
+    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>132</v>
       </c>
@@ -6586,8 +6657,20 @@
       <c r="K208" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O208">
+        <f t="shared" si="0"/>
+        <v>8.0129870129870131</v>
+      </c>
+      <c r="P208">
+        <f t="shared" si="1"/>
+        <v>16.948051948051948</v>
+      </c>
+      <c r="Q208">
+        <f t="shared" si="2"/>
+        <v>2.1150729335494329</v>
+      </c>
+    </row>
+    <row r="209" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>132</v>
       </c>
@@ -6609,8 +6692,20 @@
       <c r="K209" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O209">
+        <f t="shared" si="0"/>
+        <v>8.0194805194805188</v>
+      </c>
+      <c r="P209">
+        <f t="shared" si="1"/>
+        <v>16.948051948051948</v>
+      </c>
+      <c r="Q209">
+        <f t="shared" si="2"/>
+        <v>2.1133603238866399</v>
+      </c>
+    </row>
+    <row r="210" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>132</v>
       </c>
@@ -6632,8 +6727,20 @@
       <c r="K210" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O210">
+        <f t="shared" si="0"/>
+        <v>7.9935483870967738</v>
+      </c>
+      <c r="P210">
+        <f t="shared" si="1"/>
+        <v>16.838709677419356</v>
+      </c>
+      <c r="Q210">
+        <f t="shared" si="2"/>
+        <v>2.1065375302663436</v>
+      </c>
+    </row>
+    <row r="211" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>132</v>
       </c>
@@ -6655,8 +6762,20 @@
       <c r="K211" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O211">
+        <f t="shared" si="0"/>
+        <v>6.6497175141242941</v>
+      </c>
+      <c r="P211">
+        <f t="shared" si="1"/>
+        <v>13.728813559322035</v>
+      </c>
+      <c r="Q211">
+        <f t="shared" si="2"/>
+        <v>2.0645709430756161</v>
+      </c>
+    </row>
+    <row r="212" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>132</v>
       </c>
@@ -6678,8 +6797,28 @@
       <c r="K212" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="O212">
+        <f>C212/B212</f>
+        <v>4.7835820895522385</v>
+      </c>
+      <c r="P212">
+        <f>D212/B212</f>
+        <v>9.8208955223880601</v>
+      </c>
+      <c r="Q212">
+        <f t="shared" si="2"/>
+        <v>2.0530421216848675</v>
+      </c>
+      <c r="R212">
+        <f>E212/B212</f>
+        <v>37.940298507462686</v>
+      </c>
+      <c r="S212">
+        <f>E212/C212</f>
+        <v>7.9313572542901714</v>
+      </c>
+    </row>
+    <row r="213" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>132</v>
       </c>
@@ -6701,8 +6840,28 @@
       <c r="K213" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O213">
+        <f t="shared" ref="O213:O228" si="3">C213/B213</f>
+        <v>4.4322344322344325</v>
+      </c>
+      <c r="P213">
+        <f t="shared" ref="P213:P228" si="4">D213/B213</f>
+        <v>9.1208791208791204</v>
+      </c>
+      <c r="Q213">
+        <f t="shared" si="2"/>
+        <v>2.0578512396694215</v>
+      </c>
+      <c r="R213">
+        <f t="shared" ref="R213:R228" si="5">E213/B213</f>
+        <v>33.479853479853482</v>
+      </c>
+      <c r="S213">
+        <f t="shared" ref="S213:S228" si="6">E213/C213</f>
+        <v>7.553719008264463</v>
+      </c>
+    </row>
+    <row r="214" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>132</v>
       </c>
@@ -6724,8 +6883,28 @@
       <c r="K214" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O214">
+        <f t="shared" si="3"/>
+        <v>4.3430656934306571</v>
+      </c>
+      <c r="P214">
+        <f t="shared" si="4"/>
+        <v>9.0510948905109494</v>
+      </c>
+      <c r="Q214">
+        <f t="shared" si="2"/>
+        <v>2.0840336134453783</v>
+      </c>
+      <c r="R214">
+        <f t="shared" si="5"/>
+        <v>33.321167883211679</v>
+      </c>
+      <c r="S214">
+        <f t="shared" si="6"/>
+        <v>7.6722689075630255</v>
+      </c>
+    </row>
+    <row r="215" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>132</v>
       </c>
@@ -6747,8 +6926,28 @@
       <c r="K215" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O215">
+        <f t="shared" si="3"/>
+        <v>4.4765342960288805</v>
+      </c>
+      <c r="P215">
+        <f t="shared" si="4"/>
+        <v>9.1335740072202167</v>
+      </c>
+      <c r="Q215">
+        <f t="shared" si="2"/>
+        <v>2.0403225806451615</v>
+      </c>
+      <c r="R215">
+        <f t="shared" si="5"/>
+        <v>33.068592057761734</v>
+      </c>
+      <c r="S215">
+        <f t="shared" si="6"/>
+        <v>7.387096774193548</v>
+      </c>
+    </row>
+    <row r="216" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>132</v>
       </c>
@@ -6770,8 +6969,28 @@
       <c r="K216" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O216">
+        <f t="shared" si="3"/>
+        <v>4.2068965517241379</v>
+      </c>
+      <c r="P216">
+        <f t="shared" si="4"/>
+        <v>8.6551724137931032</v>
+      </c>
+      <c r="Q216">
+        <f t="shared" si="2"/>
+        <v>2.057377049180328</v>
+      </c>
+      <c r="R216">
+        <f t="shared" si="5"/>
+        <v>31.551724137931036</v>
+      </c>
+      <c r="S216">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>132</v>
       </c>
@@ -6793,8 +7012,28 @@
       <c r="K217" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O217">
+        <f t="shared" si="3"/>
+        <v>4.2068965517241379</v>
+      </c>
+      <c r="P217">
+        <f t="shared" si="4"/>
+        <v>8.6551724137931032</v>
+      </c>
+      <c r="Q217">
+        <f t="shared" si="2"/>
+        <v>2.057377049180328</v>
+      </c>
+      <c r="R217">
+        <f t="shared" si="5"/>
+        <v>31.551724137931036</v>
+      </c>
+      <c r="S217">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>132</v>
       </c>
@@ -6816,8 +7055,28 @@
       <c r="K218" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O218">
+        <f t="shared" si="3"/>
+        <v>4.2068965517241379</v>
+      </c>
+      <c r="P218">
+        <f t="shared" si="4"/>
+        <v>8.6551724137931032</v>
+      </c>
+      <c r="Q218">
+        <f t="shared" si="2"/>
+        <v>2.057377049180328</v>
+      </c>
+      <c r="R218">
+        <f t="shared" si="5"/>
+        <v>31.551724137931036</v>
+      </c>
+      <c r="S218">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>132</v>
       </c>
@@ -6839,8 +7098,28 @@
       <c r="K219" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O219">
+        <f t="shared" si="3"/>
+        <v>4.2068965517241379</v>
+      </c>
+      <c r="P219">
+        <f t="shared" si="4"/>
+        <v>8.6551724137931032</v>
+      </c>
+      <c r="Q219">
+        <f t="shared" si="2"/>
+        <v>2.057377049180328</v>
+      </c>
+      <c r="R219">
+        <f t="shared" si="5"/>
+        <v>31.551724137931036</v>
+      </c>
+      <c r="S219">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>132</v>
       </c>
@@ -6862,8 +7141,28 @@
       <c r="K220" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O220">
+        <f t="shared" si="3"/>
+        <v>4.2068965517241379</v>
+      </c>
+      <c r="P220">
+        <f t="shared" si="4"/>
+        <v>8.6551724137931032</v>
+      </c>
+      <c r="Q220">
+        <f t="shared" si="2"/>
+        <v>2.057377049180328</v>
+      </c>
+      <c r="R220">
+        <f t="shared" si="5"/>
+        <v>31.551724137931036</v>
+      </c>
+      <c r="S220">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>132</v>
       </c>
@@ -6885,8 +7184,28 @@
       <c r="K221" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O221">
+        <f t="shared" si="3"/>
+        <v>4.2068965517241379</v>
+      </c>
+      <c r="P221">
+        <f t="shared" si="4"/>
+        <v>8.6896551724137936</v>
+      </c>
+      <c r="Q221">
+        <f t="shared" si="2"/>
+        <v>2.0655737704918034</v>
+      </c>
+      <c r="R221">
+        <f t="shared" si="5"/>
+        <v>31.586206896551722</v>
+      </c>
+      <c r="S221">
+        <f t="shared" si="6"/>
+        <v>7.5081967213114753</v>
+      </c>
+    </row>
+    <row r="222" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>132</v>
       </c>
@@ -6908,8 +7227,28 @@
       <c r="K222" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O222">
+        <f t="shared" si="3"/>
+        <v>4.2068965517241379</v>
+      </c>
+      <c r="P222">
+        <f t="shared" si="4"/>
+        <v>8.6896551724137936</v>
+      </c>
+      <c r="Q222">
+        <f t="shared" si="2"/>
+        <v>2.0655737704918034</v>
+      </c>
+      <c r="R222">
+        <f t="shared" si="5"/>
+        <v>31.586206896551722</v>
+      </c>
+      <c r="S222">
+        <f t="shared" si="6"/>
+        <v>7.5081967213114753</v>
+      </c>
+    </row>
+    <row r="223" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>132</v>
       </c>
@@ -6931,8 +7270,28 @@
       <c r="K223" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O223">
+        <f t="shared" si="3"/>
+        <v>4.2068965517241379</v>
+      </c>
+      <c r="P223">
+        <f t="shared" si="4"/>
+        <v>8.6896551724137936</v>
+      </c>
+      <c r="Q223">
+        <f t="shared" si="2"/>
+        <v>2.0655737704918034</v>
+      </c>
+      <c r="R223">
+        <f t="shared" si="5"/>
+        <v>31.586206896551722</v>
+      </c>
+      <c r="S223">
+        <f t="shared" si="6"/>
+        <v>7.5081967213114753</v>
+      </c>
+    </row>
+    <row r="224" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>132</v>
       </c>
@@ -6954,8 +7313,28 @@
       <c r="K224" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O224">
+        <f t="shared" si="3"/>
+        <v>4.0666666666666664</v>
+      </c>
+      <c r="P224">
+        <f t="shared" si="4"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="Q224">
+        <f t="shared" si="2"/>
+        <v>2.0491803278688523</v>
+      </c>
+      <c r="R224">
+        <f t="shared" si="5"/>
+        <v>30.466666666666665</v>
+      </c>
+      <c r="S224">
+        <f t="shared" si="6"/>
+        <v>7.4918032786885247</v>
+      </c>
+    </row>
+    <row r="225" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>132</v>
       </c>
@@ -6977,8 +7356,28 @@
       <c r="K225" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O225">
+        <f t="shared" si="3"/>
+        <v>4.0666666666666664</v>
+      </c>
+      <c r="P225">
+        <f t="shared" si="4"/>
+        <v>8.3666666666666671</v>
+      </c>
+      <c r="Q225">
+        <f t="shared" si="2"/>
+        <v>2.057377049180328</v>
+      </c>
+      <c r="R225">
+        <f t="shared" si="5"/>
+        <v>30.5</v>
+      </c>
+      <c r="S225">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>132</v>
       </c>
@@ -7000,8 +7399,28 @@
       <c r="K226" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O226">
+        <f t="shared" si="3"/>
+        <v>4.0666666666666664</v>
+      </c>
+      <c r="P226">
+        <f t="shared" si="4"/>
+        <v>8.3666666666666671</v>
+      </c>
+      <c r="Q226">
+        <f t="shared" si="2"/>
+        <v>2.057377049180328</v>
+      </c>
+      <c r="R226">
+        <f t="shared" si="5"/>
+        <v>30.5</v>
+      </c>
+      <c r="S226">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>132</v>
       </c>
@@ -7023,8 +7442,28 @@
       <c r="K227" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O227">
+        <f t="shared" si="3"/>
+        <v>4.0666666666666664</v>
+      </c>
+      <c r="P227">
+        <f t="shared" si="4"/>
+        <v>8.3666666666666671</v>
+      </c>
+      <c r="Q227">
+        <f t="shared" si="2"/>
+        <v>2.057377049180328</v>
+      </c>
+      <c r="R227">
+        <f t="shared" si="5"/>
+        <v>30.5</v>
+      </c>
+      <c r="S227">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>132</v>
       </c>
@@ -7046,8 +7485,28 @@
       <c r="K228" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O228">
+        <f t="shared" si="3"/>
+        <v>4.0666666666666664</v>
+      </c>
+      <c r="P228">
+        <f t="shared" si="4"/>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="Q228">
+        <f t="shared" si="2"/>
+        <v>2.540983606557377</v>
+      </c>
+      <c r="R228">
+        <f t="shared" si="5"/>
+        <v>30.466666666666665</v>
+      </c>
+      <c r="S228">
+        <f t="shared" si="6"/>
+        <v>7.4918032786885247</v>
+      </c>
+    </row>
+    <row r="229" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>132</v>
       </c>
@@ -7070,7 +7529,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>134</v>
       </c>
@@ -7096,7 +7555,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>138</v>
       </c>
@@ -7116,7 +7575,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>138</v>
       </c>
@@ -7136,7 +7595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>148</v>
       </c>
@@ -7159,7 +7618,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="234" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>149</v>
       </c>
@@ -7170,7 +7629,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="235" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>158</v>
       </c>
@@ -7193,7 +7652,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="236" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>162</v>
       </c>
@@ -7210,7 +7669,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="237" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>162</v>
       </c>
@@ -7221,7 +7680,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="238" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>174</v>
       </c>
@@ -7232,7 +7691,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="239" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>182</v>
       </c>
@@ -7255,7 +7714,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="240" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>186</v>
       </c>
@@ -8199,7 +8658,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>818</v>
       </c>
@@ -8224,8 +8683,20 @@
       <c r="K289" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="290" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="O289">
+        <f>C289/B289</f>
+        <v>4.3934426229508201</v>
+      </c>
+      <c r="P289">
+        <f>D289/C289</f>
+        <v>2.0223880597014925</v>
+      </c>
+      <c r="Q289">
+        <f>E289/B289</f>
+        <v>33.747540983606555</v>
+      </c>
+    </row>
+    <row r="290" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>886</v>
       </c>
@@ -8250,8 +8721,20 @@
       <c r="K290" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="291" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="O290">
+        <f>C290/B290</f>
+        <v>4.2950819672131146</v>
+      </c>
+      <c r="P290">
+        <f>D290/C290</f>
+        <v>1.9763358778625955</v>
+      </c>
+      <c r="Q290">
+        <f>E290/B290</f>
+        <v>30.252459016393441</v>
+      </c>
+    </row>
+    <row r="291" spans="1:17" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>886</v>
       </c>
@@ -8262,7 +8745,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="292" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>896</v>
       </c>
@@ -8273,7 +8756,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="293" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>1024</v>
       </c>
@@ -8284,7 +8767,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="294" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>1024</v>
       </c>
@@ -8295,7 +8778,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="295" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>1024</v>
       </c>
@@ -8306,7 +8789,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="296" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>1024</v>
       </c>
@@ -8317,7 +8800,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="297" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>1024</v>
       </c>
@@ -8328,7 +8811,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="298" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>1024</v>
       </c>
@@ -8339,7 +8822,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="299" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>1024</v>
       </c>
@@ -8350,7 +8833,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="300" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>1024</v>
       </c>
@@ -8370,5 +8853,6 @@
     <sortCondition ref="E2:E300"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>